<commit_message>
Fix bugs and typos
</commit_message>
<xml_diff>
--- a/cluster algorithm/Results_clusters=3/Weight_Final.xlsx
+++ b/cluster algorithm/Results_clusters=3/Weight_Final.xlsx
@@ -361,2522 +361,2522 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337">
-        <v>22</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505">
-        <v>19</v>
+        <v>10.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>